<commit_message>
Added Test case - EC11
</commit_message>
<xml_diff>
--- a/Test Documentation.xlsx
+++ b/Test Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomto\Documents\IDEA\NewspaperApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103B046C-7F94-4B98-961E-3C3874761BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4905CEAC-1754-4BBA-ACC0-BD5E6C3B8DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="218">
   <si>
     <t>TC1</t>
   </si>
@@ -1584,6 +1584,9 @@
     <t>Feature request</t>
   </si>
   <si>
+    <t>EC11</t>
+  </si>
+  <si>
     <t>Awaiting User entity
 Implementation</t>
   </si>
@@ -1591,6 +1594,50 @@
     <t>Must refresh the
 persistence context or else
 fails</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Use setState and setValid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Check for altered fields</t>
+    </r>
+  </si>
+  <si>
+    <t>setState with
+ APPROVED and
+setContent with
+"test content"</t>
+  </si>
+  <si>
+    <t>Fields altered successfully</t>
+  </si>
+  <si>
+    <t>11. Check if Comment methods setContent and setState function as expected with valid parameters</t>
   </si>
 </sst>
 </file>
@@ -2215,7 +2262,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2849,6 +2896,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -11728,8 +11778,8 @@
   </sheetPr>
   <dimension ref="A1:K1227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89:H91"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -11826,7 +11876,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="72">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="68" t="s">
         <v>37</v>
@@ -11851,7 +11901,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="73">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="101"/>
       <c r="F7" s="101"/>
@@ -13153,7 +13203,7 @@
         <v>194</v>
       </c>
       <c r="J89" s="189" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="12" customHeight="1">
@@ -13235,7 +13285,7 @@
         <v>41</v>
       </c>
       <c r="J95" s="189" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="12" customHeight="1">
@@ -13375,40 +13425,85 @@
       <c r="I106" s="115"/>
       <c r="J106" s="100"/>
     </row>
-    <row r="107" spans="1:10">
-      <c r="D107" s="190"/>
-      <c r="E107" s="190"/>
-      <c r="F107" s="190"/>
-      <c r="I107" s="115"/>
-      <c r="J107" s="100"/>
+    <row r="107" spans="1:10" s="107" customFormat="1" ht="30.6" customHeight="1">
+      <c r="A107" s="225" t="s">
+        <v>217</v>
+      </c>
+      <c r="B107" s="226"/>
+      <c r="C107" s="226"/>
+      <c r="D107" s="226"/>
+      <c r="E107" s="226"/>
+      <c r="F107" s="226"/>
+      <c r="G107" s="226"/>
+      <c r="H107" s="226"/>
+      <c r="I107" s="226"/>
+      <c r="J107" s="227"/>
     </row>
     <row r="108" spans="1:10">
-      <c r="D108" s="190"/>
-      <c r="E108" s="190"/>
-      <c r="F108" s="190"/>
-      <c r="I108" s="115"/>
-      <c r="J108" s="100"/>
+      <c r="A108" s="188" t="s">
+        <v>210</v>
+      </c>
+      <c r="B108" s="189" t="s">
+        <v>215</v>
+      </c>
+      <c r="C108" s="119" t="s">
+        <v>170</v>
+      </c>
+      <c r="D108" s="187" t="s">
+        <v>216</v>
+      </c>
+      <c r="E108" s="187"/>
+      <c r="F108" s="187"/>
+      <c r="G108" s="119"/>
+      <c r="H108" s="187" t="s">
+        <v>216</v>
+      </c>
+      <c r="I108" s="217" t="s">
+        <v>41</v>
+      </c>
+      <c r="J108" s="187"/>
     </row>
     <row r="109" spans="1:10">
-      <c r="D109" s="190"/>
-      <c r="E109" s="190"/>
-      <c r="F109" s="190"/>
-      <c r="I109" s="115"/>
-      <c r="J109" s="100"/>
+      <c r="A109" s="188"/>
+      <c r="B109" s="187"/>
+      <c r="C109" s="121" t="s">
+        <v>165</v>
+      </c>
+      <c r="D109" s="187"/>
+      <c r="E109" s="187"/>
+      <c r="F109" s="187"/>
+      <c r="G109" s="119"/>
+      <c r="H109" s="187"/>
+      <c r="I109" s="217"/>
+      <c r="J109" s="187"/>
     </row>
     <row r="110" spans="1:10">
-      <c r="D110" s="190"/>
-      <c r="E110" s="190"/>
-      <c r="F110" s="190"/>
-      <c r="I110" s="115"/>
-      <c r="J110" s="100"/>
+      <c r="A110" s="188"/>
+      <c r="B110" s="187"/>
+      <c r="C110" s="119" t="s">
+        <v>213</v>
+      </c>
+      <c r="D110" s="187"/>
+      <c r="E110" s="187"/>
+      <c r="F110" s="187"/>
+      <c r="G110" s="119"/>
+      <c r="H110" s="187"/>
+      <c r="I110" s="217"/>
+      <c r="J110" s="187"/>
     </row>
     <row r="111" spans="1:10">
-      <c r="D111" s="190"/>
-      <c r="E111" s="190"/>
-      <c r="F111" s="190"/>
-      <c r="I111" s="115"/>
-      <c r="J111" s="100"/>
+      <c r="A111" s="188"/>
+      <c r="B111" s="187"/>
+      <c r="C111" s="228" t="s">
+        <v>214</v>
+      </c>
+      <c r="D111" s="187"/>
+      <c r="E111" s="187"/>
+      <c r="F111" s="187"/>
+      <c r="G111" s="119"/>
+      <c r="H111" s="187"/>
+      <c r="I111" s="217"/>
+      <c r="J111" s="187"/>
     </row>
     <row r="112" spans="1:10">
       <c r="D112" s="190"/>
@@ -18022,13 +18117,19 @@
       <c r="J1227" s="100"/>
     </row>
   </sheetData>
-  <mergeCells count="206">
+  <mergeCells count="208">
+    <mergeCell ref="H108:H111"/>
+    <mergeCell ref="I108:I111"/>
+    <mergeCell ref="J108:J111"/>
     <mergeCell ref="A102:A104"/>
     <mergeCell ref="B102:B104"/>
     <mergeCell ref="D102:F104"/>
     <mergeCell ref="H102:H104"/>
     <mergeCell ref="I102:I104"/>
     <mergeCell ref="J102:J104"/>
+    <mergeCell ref="A107:J107"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="A108:A111"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="H3:J3"/>
@@ -18156,16 +18257,12 @@
     <mergeCell ref="I95:I98"/>
     <mergeCell ref="J95:J98"/>
     <mergeCell ref="A101:J101"/>
-    <mergeCell ref="D109:F109"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="D111:F111"/>
     <mergeCell ref="D112:F112"/>
     <mergeCell ref="D113:F113"/>
     <mergeCell ref="D114:F114"/>
     <mergeCell ref="D105:F105"/>
     <mergeCell ref="D106:F106"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="D108:F108"/>
+    <mergeCell ref="D108:F111"/>
     <mergeCell ref="D121:F121"/>
     <mergeCell ref="D122:F122"/>
     <mergeCell ref="D123:F123"/>

</xml_diff>

<commit_message>
Added EC1 and EC12
</commit_message>
<xml_diff>
--- a/Test Documentation.xlsx
+++ b/Test Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomto\Documents\IDEA\NewspaperApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86182FE9-BDDB-43C7-9039-5FDED99E6EAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5FA398-45F6-4691-A0FC-F5A13B0AAE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="228">
   <si>
     <t>TC1</t>
   </si>
@@ -1525,9 +1525,15 @@
     <t>EC10</t>
   </si>
   <si>
+    <t>EC11</t>
+  </si>
+  <si>
     <t>Must refresh the
 persistence context or else
 fails</t>
+  </si>
+  <si>
+    <t>10. Check if Comment methods setContent and setState function as expected with valid parameters</t>
   </si>
   <si>
     <r>
@@ -1571,9 +1577,6 @@
     <t>Fields altered successfully</t>
   </si>
   <si>
-    <t>11. Check if Comment methods setContent and setState function as expected with valid parameters</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1604,7 +1607,132 @@
     <t>Added extra Comment tests</t>
   </si>
   <si>
-    <t>Commit 516177c</t>
+    <t>11. Check if a Comment's content may exceed the maximum size</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Create a valid Comment Entity with
+content size that exceeds the maximum</t>
+    </r>
+  </si>
+  <si>
+    <t>Content Size
+constraint check</t>
+  </si>
+  <si>
+    <t>Constraint Violation Exception</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Use setContent with size exceeding content</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">setContent constraint check </t>
+  </si>
+  <si>
+    <t>Runtime Exception</t>
+  </si>
+  <si>
+    <t>Thrown when persisting</t>
+  </si>
+  <si>
+    <t>EC12</t>
+  </si>
+  <si>
+    <t>12. Check if after updating a Story's name, the change is reflected in the Comment's Story</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Create a valid Comment Entity assosiaced 
+with the Story</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Alter Story's name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Refresh the Comment</t>
+    </r>
+  </si>
+  <si>
+    <t>Altered name is shown</t>
+  </si>
+  <si>
+    <t>Commit 19eb22c</t>
   </si>
 </sst>
 </file>
@@ -2229,7 +2357,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2853,6 +2981,9 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -5461,8 +5592,8 @@
   </sheetPr>
   <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -5624,19 +5755,19 @@
         <v>45115</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>184</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>107</v>
       </c>
       <c r="G13" s="121" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="17" customFormat="1" ht="30" customHeight="1">
@@ -5724,7 +5855,7 @@
   <hyperlinks>
     <hyperlink ref="G12" r:id="rId1" xr:uid="{FF85C68E-5FE4-42BD-8522-F17E18BE3D46}"/>
     <hyperlink ref="G11" r:id="rId2" location="diff-98aea50246c5a314b5ef13c39fe2b37e5a296ac3586d9caa51b5dd1958e8b5ac" xr:uid="{36E5DF57-A6B2-4A7E-81D9-8E61D006EFE9}"/>
-    <hyperlink ref="G13" r:id="rId3" xr:uid="{5E203539-7B9D-45BF-94E1-CC46496ABD1B}"/>
+    <hyperlink ref="G13" r:id="rId3" xr:uid="{ACFC7BCB-99F7-4DE4-A322-35EA24FDCC9F}"/>
   </hyperlinks>
   <pageMargins left="0.37" right="0.47" top="0.5" bottom="0.38" header="0.5" footer="0.17"/>
   <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" horizontalDpi="96" verticalDpi="96" r:id="rId4"/>
@@ -5742,8 +5873,8 @@
   </sheetPr>
   <dimension ref="A1:N1227"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -11745,8 +11876,8 @@
   </sheetPr>
   <dimension ref="A1:K1227"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="1"/>
@@ -11754,7 +11885,8 @@
     <col min="1" max="1" width="15.77734375" style="113" customWidth="1"/>
     <col min="2" max="2" width="18.109375" style="99" customWidth="1"/>
     <col min="3" max="3" width="42.44140625" style="99" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="99"/>
+    <col min="4" max="4" width="9.21875" style="99" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="99"/>
     <col min="6" max="6" width="15.44140625" style="99" customWidth="1"/>
     <col min="7" max="7" width="18.44140625" style="99" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="32.88671875" style="99" customWidth="1"/>
@@ -11843,7 +11975,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="72">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="68" t="s">
         <v>37</v>
@@ -11868,7 +12000,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="73">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E7" s="100"/>
       <c r="F7" s="100"/>
@@ -13172,7 +13304,7 @@
         <v>41</v>
       </c>
       <c r="J89" s="188" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="12" customHeight="1">
@@ -13254,7 +13386,7 @@
         <v>41</v>
       </c>
       <c r="J95" s="188" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="12" customHeight="1">
@@ -13275,7 +13407,7 @@
       <c r="A97" s="187"/>
       <c r="B97" s="186"/>
       <c r="C97" s="120" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D97" s="186"/>
       <c r="E97" s="186"/>
@@ -13315,7 +13447,7 @@
     </row>
     <row r="101" spans="1:10" s="106" customFormat="1" ht="30.6" customHeight="1">
       <c r="A101" s="220" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B101" s="221"/>
       <c r="C101" s="221"/>
@@ -13332,19 +13464,19 @@
         <v>201</v>
       </c>
       <c r="B102" s="188" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C102" s="118" t="s">
         <v>170</v>
       </c>
       <c r="D102" s="186" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E102" s="186"/>
       <c r="F102" s="186"/>
       <c r="G102" s="118"/>
       <c r="H102" s="186" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="I102" s="216" t="s">
         <v>41</v>
@@ -13369,7 +13501,7 @@
       <c r="A104" s="187"/>
       <c r="B104" s="186"/>
       <c r="C104" s="118" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D104" s="186"/>
       <c r="E104" s="186"/>
@@ -13383,7 +13515,7 @@
       <c r="A105" s="187"/>
       <c r="B105" s="186"/>
       <c r="C105" s="223" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D105" s="186"/>
       <c r="E105" s="186"/>
@@ -13402,138 +13534,255 @@
     </row>
     <row r="107" spans="1:10" s="106" customFormat="1" ht="10.199999999999999"/>
     <row r="108" spans="1:10">
-      <c r="H108"/>
-      <c r="I108"/>
-      <c r="J108"/>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="H109"/>
-      <c r="I109"/>
-      <c r="J109"/>
+      <c r="A108" s="151" t="s">
+        <v>213</v>
+      </c>
+      <c r="B108" s="152"/>
+      <c r="C108" s="152"/>
+      <c r="D108" s="152"/>
+      <c r="E108" s="152"/>
+      <c r="F108" s="152"/>
+      <c r="G108" s="152"/>
+      <c r="H108" s="152"/>
+      <c r="I108" s="152"/>
+      <c r="J108" s="153"/>
+    </row>
+    <row r="109" spans="1:10" ht="27.6">
+      <c r="A109" s="187" t="s">
+        <v>202</v>
+      </c>
+      <c r="B109" s="188" t="s">
+        <v>215</v>
+      </c>
+      <c r="C109" s="120" t="s">
+        <v>214</v>
+      </c>
+      <c r="D109" s="186" t="s">
+        <v>216</v>
+      </c>
+      <c r="E109" s="186"/>
+      <c r="F109" s="186"/>
+      <c r="G109" s="118"/>
+      <c r="H109" s="188" t="s">
+        <v>216</v>
+      </c>
+      <c r="I109" s="216" t="s">
+        <v>41</v>
+      </c>
+      <c r="J109" s="224" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="110" spans="1:10">
-      <c r="H110"/>
-      <c r="I110"/>
-      <c r="J110"/>
+      <c r="A110" s="187"/>
+      <c r="B110" s="188"/>
+      <c r="C110" s="120" t="s">
+        <v>165</v>
+      </c>
+      <c r="D110" s="186"/>
+      <c r="E110" s="186"/>
+      <c r="F110" s="186"/>
+      <c r="G110" s="118"/>
+      <c r="H110" s="188"/>
+      <c r="I110" s="216"/>
+      <c r="J110" s="188"/>
     </row>
     <row r="111" spans="1:10">
-      <c r="H111"/>
-      <c r="I111"/>
-      <c r="J111"/>
+      <c r="A111" s="187"/>
+      <c r="B111" s="190" t="s">
+        <v>116</v>
+      </c>
+      <c r="C111" s="190"/>
+      <c r="D111" s="190"/>
+      <c r="E111" s="190"/>
+      <c r="F111" s="190"/>
+      <c r="G111" s="190"/>
+      <c r="H111" s="190"/>
+      <c r="I111" s="190"/>
+      <c r="J111" s="190"/>
     </row>
     <row r="112" spans="1:10">
-      <c r="D112" s="189"/>
-      <c r="E112" s="189"/>
-      <c r="F112" s="189"/>
-      <c r="I112" s="114"/>
-      <c r="J112" s="99"/>
-    </row>
-    <row r="113" spans="4:10">
-      <c r="D113" s="189"/>
-      <c r="E113" s="189"/>
-      <c r="F113" s="189"/>
-      <c r="I113" s="114"/>
-      <c r="J113" s="99"/>
-    </row>
-    <row r="114" spans="4:10">
+      <c r="A112" s="187"/>
+      <c r="B112" s="188" t="s">
+        <v>218</v>
+      </c>
+      <c r="C112" s="118" t="s">
+        <v>170</v>
+      </c>
+      <c r="D112" s="186" t="s">
+        <v>219</v>
+      </c>
+      <c r="E112" s="186"/>
+      <c r="F112" s="186"/>
+      <c r="G112" s="118"/>
+      <c r="H112" s="186" t="s">
+        <v>219</v>
+      </c>
+      <c r="I112" s="216" t="s">
+        <v>41</v>
+      </c>
+      <c r="J112" s="186"/>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="187"/>
+      <c r="B113" s="186"/>
+      <c r="C113" s="118" t="s">
+        <v>217</v>
+      </c>
+      <c r="D113" s="186"/>
+      <c r="E113" s="186"/>
+      <c r="F113" s="186"/>
+      <c r="G113" s="118"/>
+      <c r="H113" s="186"/>
+      <c r="I113" s="216"/>
+      <c r="J113" s="186"/>
+    </row>
+    <row r="114" spans="1:10">
       <c r="D114" s="189"/>
       <c r="E114" s="189"/>
       <c r="F114" s="189"/>
       <c r="I114" s="114"/>
       <c r="J114" s="99"/>
     </row>
-    <row r="115" spans="4:10">
+    <row r="115" spans="1:10">
       <c r="D115" s="189"/>
       <c r="E115" s="189"/>
       <c r="F115" s="189"/>
       <c r="I115" s="114"/>
       <c r="J115" s="99"/>
     </row>
-    <row r="116" spans="4:10">
-      <c r="D116" s="189"/>
-      <c r="E116" s="189"/>
-      <c r="F116" s="189"/>
-      <c r="I116" s="114"/>
-      <c r="J116" s="99"/>
-    </row>
-    <row r="117" spans="4:10">
-      <c r="D117" s="189"/>
-      <c r="E117" s="189"/>
-      <c r="F117" s="189"/>
-      <c r="I117" s="114"/>
-      <c r="J117" s="99"/>
-    </row>
-    <row r="118" spans="4:10">
-      <c r="D118" s="189"/>
-      <c r="E118" s="189"/>
-      <c r="F118" s="189"/>
-      <c r="I118" s="114"/>
-      <c r="J118" s="99"/>
-    </row>
-    <row r="119" spans="4:10">
-      <c r="D119" s="189"/>
-      <c r="E119" s="189"/>
-      <c r="F119" s="189"/>
-      <c r="I119" s="114"/>
-      <c r="J119" s="99"/>
-    </row>
-    <row r="120" spans="4:10">
-      <c r="D120" s="189"/>
-      <c r="E120" s="189"/>
-      <c r="F120" s="189"/>
-      <c r="I120" s="114"/>
-      <c r="J120" s="99"/>
-    </row>
-    <row r="121" spans="4:10">
+    <row r="116" spans="1:10">
+      <c r="A116" s="151" t="s">
+        <v>222</v>
+      </c>
+      <c r="B116" s="152"/>
+      <c r="C116" s="152"/>
+      <c r="D116" s="152"/>
+      <c r="E116" s="152"/>
+      <c r="F116" s="152"/>
+      <c r="G116" s="152"/>
+      <c r="H116" s="152"/>
+      <c r="I116" s="152"/>
+      <c r="J116" s="153"/>
+    </row>
+    <row r="117" spans="1:10" ht="27.6">
+      <c r="A117" s="187" t="s">
+        <v>221</v>
+      </c>
+      <c r="B117" s="188" t="s">
+        <v>199</v>
+      </c>
+      <c r="C117" s="120" t="s">
+        <v>223</v>
+      </c>
+      <c r="D117" s="186" t="s">
+        <v>226</v>
+      </c>
+      <c r="E117" s="186"/>
+      <c r="F117" s="186"/>
+      <c r="G117" s="118"/>
+      <c r="H117" s="186" t="s">
+        <v>226</v>
+      </c>
+      <c r="I117" s="216" t="s">
+        <v>41</v>
+      </c>
+      <c r="J117" s="188" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="187"/>
+      <c r="B118" s="186"/>
+      <c r="C118" s="120" t="s">
+        <v>165</v>
+      </c>
+      <c r="D118" s="186"/>
+      <c r="E118" s="186"/>
+      <c r="F118" s="186"/>
+      <c r="G118" s="118"/>
+      <c r="H118" s="186"/>
+      <c r="I118" s="216"/>
+      <c r="J118" s="186"/>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="187"/>
+      <c r="B119" s="186"/>
+      <c r="C119" s="120" t="s">
+        <v>224</v>
+      </c>
+      <c r="D119" s="186"/>
+      <c r="E119" s="186"/>
+      <c r="F119" s="186"/>
+      <c r="G119" s="118"/>
+      <c r="H119" s="186"/>
+      <c r="I119" s="216"/>
+      <c r="J119" s="186"/>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" s="187"/>
+      <c r="B120" s="186"/>
+      <c r="C120" s="120" t="s">
+        <v>225</v>
+      </c>
+      <c r="D120" s="186"/>
+      <c r="E120" s="186"/>
+      <c r="F120" s="186"/>
+      <c r="G120" s="118"/>
+      <c r="H120" s="186"/>
+      <c r="I120" s="216"/>
+      <c r="J120" s="186"/>
+    </row>
+    <row r="121" spans="1:10">
       <c r="D121" s="189"/>
       <c r="E121" s="189"/>
       <c r="F121" s="189"/>
       <c r="I121" s="114"/>
       <c r="J121" s="99"/>
     </row>
-    <row r="122" spans="4:10">
+    <row r="122" spans="1:10">
       <c r="D122" s="189"/>
       <c r="E122" s="189"/>
       <c r="F122" s="189"/>
       <c r="I122" s="114"/>
       <c r="J122" s="99"/>
     </row>
-    <row r="123" spans="4:10">
+    <row r="123" spans="1:10">
       <c r="D123" s="189"/>
       <c r="E123" s="189"/>
       <c r="F123" s="189"/>
       <c r="I123" s="114"/>
       <c r="J123" s="99"/>
     </row>
-    <row r="124" spans="4:10">
+    <row r="124" spans="1:10">
       <c r="D124" s="189"/>
       <c r="E124" s="189"/>
       <c r="F124" s="189"/>
       <c r="I124" s="114"/>
       <c r="J124" s="99"/>
     </row>
-    <row r="125" spans="4:10">
+    <row r="125" spans="1:10">
       <c r="D125" s="189"/>
       <c r="E125" s="189"/>
       <c r="F125" s="189"/>
       <c r="I125" s="114"/>
       <c r="J125" s="99"/>
     </row>
-    <row r="126" spans="4:10">
+    <row r="126" spans="1:10">
       <c r="D126" s="189"/>
       <c r="E126" s="189"/>
       <c r="F126" s="189"/>
       <c r="I126" s="114"/>
       <c r="J126" s="99"/>
     </row>
-    <row r="127" spans="4:10">
+    <row r="127" spans="1:10">
       <c r="D127" s="189"/>
       <c r="E127" s="189"/>
       <c r="F127" s="189"/>
       <c r="I127" s="114"/>
       <c r="J127" s="99"/>
     </row>
-    <row r="128" spans="4:10">
+    <row r="128" spans="1:10">
       <c r="D128" s="189"/>
       <c r="E128" s="189"/>
       <c r="F128" s="189"/>
@@ -18033,10 +18282,30 @@
       <c r="J1227" s="99"/>
     </row>
   </sheetData>
-  <mergeCells count="200">
+  <mergeCells count="213">
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="D112:F113"/>
+    <mergeCell ref="H112:H113"/>
+    <mergeCell ref="I112:I113"/>
+    <mergeCell ref="J112:J113"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="A116:J116"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="D117:F120"/>
+    <mergeCell ref="H117:H120"/>
+    <mergeCell ref="I117:I120"/>
+    <mergeCell ref="J117:J120"/>
     <mergeCell ref="H102:H105"/>
     <mergeCell ref="I102:I105"/>
     <mergeCell ref="J102:J105"/>
+    <mergeCell ref="A108:J108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="D109:F110"/>
+    <mergeCell ref="H109:H110"/>
+    <mergeCell ref="I109:I110"/>
+    <mergeCell ref="J109:J110"/>
+    <mergeCell ref="B111:J111"/>
     <mergeCell ref="A101:J101"/>
     <mergeCell ref="B102:B105"/>
     <mergeCell ref="A102:A105"/>
@@ -18166,8 +18435,6 @@
     <mergeCell ref="H95:H98"/>
     <mergeCell ref="I95:I98"/>
     <mergeCell ref="J95:J98"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="D113:F113"/>
     <mergeCell ref="D114:F114"/>
     <mergeCell ref="D106:F106"/>
     <mergeCell ref="D102:F105"/>
@@ -18178,11 +18445,6 @@
     <mergeCell ref="D125:F125"/>
     <mergeCell ref="D126:F126"/>
     <mergeCell ref="D115:F115"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="D119:F119"/>
-    <mergeCell ref="D120:F120"/>
     <mergeCell ref="D143:F143"/>
     <mergeCell ref="D144:F144"/>
     <mergeCell ref="D133:F133"/>
@@ -18246,7 +18508,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>

</xml_diff>

<commit_message>
Added EC11 and EC12
</commit_message>
<xml_diff>
--- a/Test Documentation.xlsx
+++ b/Test Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomto\Documents\IDEA\NewspaperApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5FA398-45F6-4691-A0FC-F5A13B0AAE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AA1D1A-261B-484E-AD3C-262A9D6649C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="821" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="821" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="97" r:id="rId1"/>
@@ -1732,7 +1732,7 @@
     <t>Altered name is shown</t>
   </si>
   <si>
-    <t>Commit 19eb22c</t>
+    <t>Commit 9568a9e</t>
   </si>
 </sst>
 </file>
@@ -5592,8 +5592,8 @@
   </sheetPr>
   <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -5855,7 +5855,7 @@
   <hyperlinks>
     <hyperlink ref="G12" r:id="rId1" xr:uid="{FF85C68E-5FE4-42BD-8522-F17E18BE3D46}"/>
     <hyperlink ref="G11" r:id="rId2" location="diff-98aea50246c5a314b5ef13c39fe2b37e5a296ac3586d9caa51b5dd1958e8b5ac" xr:uid="{36E5DF57-A6B2-4A7E-81D9-8E61D006EFE9}"/>
-    <hyperlink ref="G13" r:id="rId3" xr:uid="{ACFC7BCB-99F7-4DE4-A322-35EA24FDCC9F}"/>
+    <hyperlink ref="G13" r:id="rId3" xr:uid="{4E3BB830-C43D-4E7A-804E-D53909EE12B5}"/>
   </hyperlinks>
   <pageMargins left="0.37" right="0.47" top="0.5" bottom="0.38" header="0.5" footer="0.17"/>
   <pageSetup paperSize="9" scale="84" fitToHeight="0" orientation="landscape" horizontalDpi="96" verticalDpi="96" r:id="rId4"/>
@@ -11876,7 +11876,7 @@
   </sheetPr>
   <dimension ref="A1:K1227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>